<commit_message>
AIP-1322 AIP-1382 Updated the excel sheet data for cabling
</commit_message>
<xml_diff>
--- a/AutoFirmwareUpgrade/CashelFirmwareAutomatedTest/TestDataFiles/FR_DISPATCHRMS_DATASET_18Channel/1U3I3I3I_phC.xlsx
+++ b/AutoFirmwareUpgrade/CashelFirmwareAutomatedTest/TestDataFiles/FR_DISPATCHRMS_DATASET_18Channel/1U3I3I3I_phC.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE29AEC-699A-41BA-B07F-C1729B0256AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71FB732-4AD8-4E54-9425-5104FAFAFB6A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StandaloneParameters" sheetId="6" r:id="rId1"/>
@@ -9925,7 +9925,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">

</xml_diff>